<commit_message>
Update sleep diary data (new version)
</commit_message>
<xml_diff>
--- a/data/baseline+diary/001_-_Full_Utregning.xlsx
+++ b/data/baseline+diary/001_-_Full_Utregning.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saa054\Dropbox\mw-sleep-analysis-simplified\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso-my.sharepoint.com/personal/saa054_uit_no/Documents/0 - Forskerlinjen/.2--MW_Sleep-Article/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CBCD9A-EFC7-4C9E-88C6-4A4EF98E0672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{D01057B3-A17F-4BCC-9FD3-6F8888AEA328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07976FBE-6009-4780-91B4-9D7A65D4E1ED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{AD6D089E-9814-4872-BBFB-296E4CC5E2AD}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" activeTab="3" xr2:uid="{AD6D089E-9814-4872-BBFB-296E4CC5E2AD}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="4" r:id="rId1"/>
     <sheet name="Sleep Quiz" sheetId="1" r:id="rId2"/>
     <sheet name="Sleep Diary" sheetId="3" r:id="rId3"/>
-    <sheet name="PANAS" sheetId="2" r:id="rId4"/>
-    <sheet name="Feedback-comments" sheetId="5" r:id="rId5"/>
+    <sheet name="sleepdiary2" sheetId="6" r:id="rId4"/>
+    <sheet name="PANAS" sheetId="2" r:id="rId5"/>
+    <sheet name="Feedback-comments" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="295">
   <si>
     <t>2 - Fatigue</t>
   </si>
@@ -128,6 +129,20 @@
     <t>Q1 (1)</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C4)</t>
+    </r>
+  </si>
+  <si>
     <t>Positiv SUM</t>
   </si>
   <si>
@@ -149,6 +164,20 @@
     <t>Q1 (3)</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C2a)</t>
+    </r>
+  </si>
+  <si>
     <t>Q4</t>
   </si>
   <si>
@@ -164,9 +193,37 @@
     <t>Q5</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C4)</t>
+    </r>
+  </si>
+  <si>
     <t>Q6</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C3)</t>
+    </r>
+  </si>
+  <si>
     <t>Q7</t>
   </si>
   <si>
@@ -176,67 +233,263 @@
     <t>SUM</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C2b)</t>
+    </r>
+  </si>
+  <si>
     <t>Q9</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Q10/3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
     <t>Q10</t>
   </si>
   <si>
+    <r>
+      <t>Q10/4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C2</t>
   </si>
   <si>
     <t>Q11</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
     <t>Q12</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
     <t>Q13</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
     <t>Q14</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C6</t>
   </si>
   <si>
     <t>Q15</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C7</t>
   </si>
   <si>
     <t>Q16</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q10/11 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C5)</t>
+    </r>
+  </si>
+  <si>
     <t>C Sum</t>
   </si>
   <si>
     <t>Q17</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q11 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C1)</t>
+    </r>
+  </si>
+  <si>
     <t>Sum Calc</t>
   </si>
   <si>
     <t>Q18</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q12/1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C6)</t>
+    </r>
+  </si>
+  <si>
     <t>Q19</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Q12/2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C7)</t>
+    </r>
+  </si>
+  <si>
     <t>Q20</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Q13 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(C7)</t>
+    </r>
   </si>
   <si>
     <t>Gruppe</t>
@@ -1327,278 +1580,44 @@
     <t>Quiz feil</t>
   </si>
   <si>
+    <t>Hvilke spørsmål?</t>
+  </si>
+  <si>
     <t>Hvilket spørsmål?</t>
   </si>
   <si>
     <t>Forskjell</t>
   </si>
   <si>
-    <r>
-      <t>Q6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (C4)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C2a)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C4)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C3)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C2b)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Q10/4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/6 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/7 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/9 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q10/11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q12/1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C6)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q12/2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C7)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Q13 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(C7)</t>
-    </r>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>q8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1642,12 +1661,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1938,7 +1951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2032,6 +2045,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2164,9 +2178,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2204,7 +2218,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2310,7 +2324,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2452,7 +2466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2477,89 +2491,89 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="50"/>
       <c r="D1" s="62" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="37">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="37">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="44" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="37">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="37">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="37">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="78">
         <v>44263</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="44" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="37">
@@ -2569,7 +2583,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="H8" s="80">
         <f>((E8/0.6)/100)+D8</f>
@@ -2578,19 +2592,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="78">
         <v>44270</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="44" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="37">
@@ -2600,7 +2614,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="H10" s="80">
         <f>((E10/0.6)/100)+D10</f>
@@ -2609,174 +2623,174 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="44" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C11" s="46"/>
       <c r="D11" s="37">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="44" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="37"/>
       <c r="F12" s="60" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="44" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C13" s="46"/>
       <c r="D13" s="42" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="C14" s="46"/>
       <c r="D14" s="37">
         <v>5</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B15" s="68"/>
       <c r="C15" s="62" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="D15" s="63"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="64"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C17" s="41" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="D17" s="43">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C18" s="41" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D18" s="15">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="44" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="15">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="44" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="66"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C21" s="41" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="D21" s="65">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22" s="41" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D22" s="42">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="44" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="66"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C24" s="41" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="D24" s="65">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="51" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D25" s="42">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="44" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="C26" s="46"/>
       <c r="D26" s="37">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="44" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C27" s="45"/>
       <c r="D27" s="14">
@@ -2784,23 +2798,23 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B28" s="62"/>
       <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="44" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C29" s="46"/>
       <c r="D29" s="53" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="E29" s="53"/>
       <c r="F29" s="53"/>
@@ -2814,7 +2828,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="44" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C30" s="46"/>
       <c r="D30" s="53"/>
@@ -2830,7 +2844,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="44" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C31" s="46"/>
       <c r="D31" s="53"/>
@@ -2846,7 +2860,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="44" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C32" s="46"/>
       <c r="D32" s="53"/>
@@ -2862,14 +2876,14 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B33" s="62"/>
       <c r="C33" s="69"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="44" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C34" s="46"/>
       <c r="D34" s="53"/>
@@ -2885,7 +2899,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="44" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C35" s="46"/>
       <c r="D35" s="53"/>
@@ -2901,7 +2915,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" s="44" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C36" s="46"/>
       <c r="D36" s="53"/>
@@ -2917,7 +2931,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="44" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C37" s="46"/>
       <c r="D37" s="53"/>
@@ -2942,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1222C293-5060-48AA-A12A-214EAB2AD1B7}">
   <dimension ref="A1:AE115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2979,7 +2993,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -3006,7 +3020,7 @@
     </row>
     <row r="2" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>7</v>
@@ -3069,7 +3083,7 @@
     </row>
     <row r="3" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
@@ -3094,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>268</v>
+        <v>22</v>
       </c>
       <c r="O3" s="11">
         <v>21</v>
@@ -3123,7 +3137,7 @@
         <v>4</v>
       </c>
       <c r="Z3" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB3" s="10" t="s">
         <v>20</v>
@@ -3134,40 +3148,40 @@
     </row>
     <row r="4" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="9">
         <v>2</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="9">
         <v>0</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U4" s="11">
         <v>2</v>
@@ -3177,7 +3191,7 @@
         <v>2</v>
       </c>
       <c r="X4" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y4" s="15">
         <v>1</v>
@@ -3188,7 +3202,7 @@
       </c>
       <c r="AA4"/>
       <c r="AB4" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC4" s="11">
         <v>2</v>
@@ -3196,7 +3210,7 @@
     </row>
     <row r="5" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="11">
         <v>21</v>
@@ -3205,25 +3219,25 @@
         <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="9">
         <v>3</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="9">
         <v>0</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L5" s="9">
         <v>0</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>269</v>
+        <v>30</v>
       </c>
       <c r="O5" s="11">
         <v>30</v>
@@ -3237,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U5" s="11">
         <v>3</v>
@@ -3247,7 +3261,7 @@
         <v>2</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Y5" s="15">
         <v>2</v>
@@ -3255,7 +3269,7 @@
       <c r="Z5"/>
       <c r="AA5"/>
       <c r="AB5" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC5" s="11">
         <v>1</v>
@@ -3263,7 +3277,7 @@
     </row>
     <row r="6" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="11">
         <v>6</v>
@@ -3272,19 +3286,19 @@
         <v>0</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F6" s="9">
         <v>4</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I6" s="9">
         <v>0</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6" s="9">
         <v>0</v>
@@ -3299,10 +3313,10 @@
         <v>13</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U6" s="11">
         <v>4</v>
@@ -3312,17 +3326,17 @@
         <v>4</v>
       </c>
       <c r="X6" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Y6" s="15">
         <v>2</v>
       </c>
       <c r="Z6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AA6"/>
       <c r="AB6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AC6" s="20">
         <f>SUM(AC3:AC5)</f>
@@ -3331,32 +3345,32 @@
     </row>
     <row r="7" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="11">
         <v>8</v>
       </c>
       <c r="C7" s="11"/>
       <c r="E7" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="9">
         <v>3</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I7" s="9">
         <v>1</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L7" s="9">
         <v>0</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>270</v>
+        <v>36</v>
       </c>
       <c r="O7" s="11">
         <v>6</v>
@@ -3373,7 +3387,7 @@
         <v>94.117647058823522</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U7" s="11">
         <v>3</v>
@@ -3383,7 +3397,7 @@
         <v>3</v>
       </c>
       <c r="X7" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Y7" s="15">
         <v>3</v>
@@ -3396,32 +3410,32 @@
     </row>
     <row r="8" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="11">
         <v>8</v>
       </c>
       <c r="C8" s="11"/>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F8" s="9">
         <v>3</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I8" s="9">
         <v>0</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L8" s="9">
         <v>1</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>271</v>
+        <v>38</v>
       </c>
       <c r="O8" s="11">
         <v>8</v>
@@ -3434,7 +3448,7 @@
         <v>8</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U8" s="11">
         <v>1</v>
@@ -3444,7 +3458,7 @@
         <v>4</v>
       </c>
       <c r="X8" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Y8" s="15">
         <v>1</v>
@@ -3454,26 +3468,26 @@
     </row>
     <row r="9" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B9" s="11">
         <v>9</v>
       </c>
       <c r="C9" s="71"/>
       <c r="E9" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F9" s="9">
         <v>1</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I9" s="9">
         <v>0</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L9" s="9">
         <v>0</v>
@@ -3485,10 +3499,10 @@
         <v>16</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="U9" s="11">
         <v>1</v>
@@ -3498,7 +3512,7 @@
         <v>4</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="Y9" s="15">
         <v>1</v>
@@ -3511,26 +3525,26 @@
         <v>7</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F10" s="9">
         <v>2</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I10" s="9">
         <v>0</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L10" s="22">
         <f>SUM(L3:L9)</f>
         <v>2</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>272</v>
+        <v>42</v>
       </c>
       <c r="O10" s="11">
         <v>1</v>
@@ -3544,14 +3558,14 @@
         <v>1</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V10" s="20">
         <f>SUM(V3:V9)/7</f>
         <v>3.2857142857142856</v>
       </c>
       <c r="X10" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="Y10" s="15">
         <v>1</v>
@@ -3561,33 +3575,33 @@
     </row>
     <row r="11" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F11" s="9">
         <v>6</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I11" s="23">
         <f>SUM(I3:I10)</f>
         <v>2</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L11" s="22">
         <f>SUM(GESTEP(L10,0),GESTEP(L10,8),GESTEP(L10,15),GESTEP(L10,22))</f>
         <v>1</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>273</v>
+        <v>44</v>
       </c>
       <c r="O11" s="11">
         <v>2</v>
@@ -3597,7 +3611,7 @@
         <v>1</v>
       </c>
       <c r="X11" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="Y11" s="15">
         <v>4</v>
@@ -3607,7 +3621,7 @@
     </row>
     <row r="12" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" s="70">
         <v>0</v>
@@ -3621,14 +3635,14 @@
         <v>3.1111111111111112</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I12" s="22">
         <f>SUM(GESTEP(I11,0),GESTEP(I11,6),GESTEP(I11,11),GESTEP(I11,13),GESTEP(I11,16))</f>
         <v>1</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>274</v>
+        <v>45</v>
       </c>
       <c r="O12" s="11">
         <v>1</v>
@@ -3638,14 +3652,14 @@
         <v>0</v>
       </c>
       <c r="Q12" s="38" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="R12" s="24">
         <f>P20</f>
         <v>0</v>
       </c>
       <c r="X12" s="14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="Y12" s="15">
         <v>3</v>
@@ -3655,7 +3669,7 @@
     </row>
     <row r="13" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="N13" s="10" t="s">
-        <v>275</v>
+        <v>48</v>
       </c>
       <c r="O13" s="11">
         <v>1</v>
@@ -3665,14 +3679,14 @@
         <v>0</v>
       </c>
       <c r="Q13" s="38" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="R13" s="24" cm="1">
         <f t="array" ref="R13">_xlfn.IFS(Q10=0,0,Q10&lt;=2,1,Q10&lt;=4,2,Q10&lt;=6,3)</f>
         <v>1</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="Y13" s="15">
         <v>4</v>
@@ -3682,7 +3696,7 @@
     </row>
     <row r="14" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="N14" s="10" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="O14" s="11">
         <v>1</v>
@@ -3692,14 +3706,14 @@
         <v>0</v>
       </c>
       <c r="Q14" s="38" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="R14" s="24">
         <f>Q5</f>
         <v>0</v>
       </c>
       <c r="X14" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="Y14" s="15">
         <v>4</v>
@@ -3709,7 +3723,7 @@
     </row>
     <row r="15" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="N15" s="10" t="s">
-        <v>277</v>
+        <v>54</v>
       </c>
       <c r="O15" s="11">
         <v>1</v>
@@ -3719,14 +3733,14 @@
         <v>0</v>
       </c>
       <c r="Q15" s="38" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="R15" s="24" cm="1">
         <f t="array" ref="R15">_xlfn.IFS(R7&gt;=85,0,R7&gt;=75,1,R7&gt;=65,2,R7&lt;=65,3)</f>
         <v>0</v>
       </c>
       <c r="X15" s="17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="Y15" s="15">
         <v>1</v>
@@ -3736,7 +3750,7 @@
     </row>
     <row r="16" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="N16" s="10" t="s">
-        <v>278</v>
+        <v>57</v>
       </c>
       <c r="O16" s="11">
         <v>1</v>
@@ -3746,14 +3760,14 @@
         <v>0</v>
       </c>
       <c r="Q16" s="38" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="R16" s="24" cm="1">
         <f t="array" ref="R16">_xlfn.IFS(Q21=0,0,Q21&gt;=1,1,Q21&gt;=10,2,Q21&gt;=19,3)</f>
         <v>1</v>
       </c>
       <c r="X16" s="14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="Y16" s="15">
         <v>3</v>
@@ -3763,10 +3777,10 @@
     </row>
     <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>279</v>
+        <v>60</v>
       </c>
       <c r="O17" s="11">
         <v>1</v>
@@ -3776,14 +3790,14 @@
         <v>0</v>
       </c>
       <c r="Q17" s="38" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="R17" s="24">
         <f>P21</f>
         <v>0</v>
       </c>
       <c r="X17" s="17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="Y17" s="15">
         <v>3</v>
@@ -3793,7 +3807,7 @@
     </row>
     <row r="18" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N18" s="10" t="s">
-        <v>280</v>
+        <v>63</v>
       </c>
       <c r="O18" s="11">
         <v>1</v>
@@ -3803,14 +3817,14 @@
         <v>0</v>
       </c>
       <c r="Q18" s="38" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="R18" s="24" cm="1">
         <f t="array" ref="R18">_xlfn.IFS(Q23=0,0,Q23&lt;=2,1,Q23&lt;=4,2,Q23&lt;=6,3)</f>
         <v>0</v>
       </c>
       <c r="X18" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="Y18" s="15">
         <v>5</v>
@@ -3820,7 +3834,7 @@
     </row>
     <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N19" s="10" t="s">
-        <v>281</v>
+        <v>66</v>
       </c>
       <c r="O19" s="11">
         <v>1</v>
@@ -3830,14 +3844,14 @@
         <v>0</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="R19" s="20">
         <f>SUM(R12:R18)</f>
         <v>2</v>
       </c>
       <c r="X19" s="14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="Y19" s="15">
         <v>4</v>
@@ -3847,7 +3861,7 @@
     </row>
     <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N20" s="10" t="s">
-        <v>282</v>
+        <v>69</v>
       </c>
       <c r="O20" s="11">
         <v>1</v>
@@ -3857,10 +3871,10 @@
         <v>0</v>
       </c>
       <c r="Q20" s="6" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="X20" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="Y20" s="15">
         <v>1</v>
@@ -3870,7 +3884,7 @@
     </row>
     <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N21" s="10" t="s">
-        <v>283</v>
+        <v>72</v>
       </c>
       <c r="O21" s="11">
         <v>1</v>
@@ -3884,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="X21" s="14" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="Y21" s="15">
         <v>4</v>
@@ -3893,7 +3907,7 @@
     </row>
     <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="N22" s="10" t="s">
-        <v>284</v>
+        <v>74</v>
       </c>
       <c r="O22" s="11">
         <v>1</v>
@@ -3906,7 +3920,7 @@
         <v>16</v>
       </c>
       <c r="X22" s="17" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="Y22" s="15">
         <v>1</v>
@@ -3914,7 +3928,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="N23" s="10" t="s">
-        <v>285</v>
+        <v>76</v>
       </c>
       <c r="O23" s="11">
         <v>1</v>
@@ -3930,15 +3944,15 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="57" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B41" s="57"/>
     </row>
@@ -3947,7 +3961,7 @@
         <v>20</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="C42" s="58"/>
       <c r="D42" s="58"/>
@@ -3964,10 +3978,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="C43" s="58"/>
       <c r="D43" s="58"/>
@@ -3979,10 +3993,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" s="58" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C44" s="58"/>
       <c r="D44" s="58"/>
@@ -3994,10 +4008,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B45" s="58" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="C45" s="58"/>
       <c r="D45" s="58"/>
@@ -4012,10 +4026,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B46" s="58" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="C46" s="58"/>
       <c r="D46" s="58"/>
@@ -4030,10 +4044,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B47" s="58" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C47" s="58"/>
       <c r="D47" s="58"/>
@@ -4048,10 +4062,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B48" s="58" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C48" s="58"/>
       <c r="D48" s="58"/>
@@ -4066,10 +4080,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="58"/>
@@ -4084,10 +4098,10 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="59" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="C51" s="59"/>
       <c r="D51" s="59"/>
@@ -4095,10 +4109,10 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="39" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B52" s="58" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="C52" s="58"/>
       <c r="D52" s="58"/>
@@ -4107,10 +4121,10 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B53" s="58" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C53" s="58"/>
       <c r="D53" s="58"/>
@@ -4118,20 +4132,20 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B54" s="58" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="C54" s="58"/>
       <c r="D54" s="58"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="C55" s="58"/>
       <c r="D55" s="58"/>
@@ -4143,10 +4157,10 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B56" s="58" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="C56" s="58"/>
       <c r="D56" s="58"/>
@@ -4157,10 +4171,10 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B57" s="58" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="C57" s="58"/>
       <c r="D57" s="58"/>
@@ -4175,10 +4189,10 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B58" s="58" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="C58" s="58"/>
       <c r="D58" s="58"/>
@@ -4192,10 +4206,10 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B59" s="58" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="C59" s="58"/>
       <c r="D59" s="58"/>
@@ -4208,10 +4222,10 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B60" s="58" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C60" s="58"/>
       <c r="D60" s="58"/>
@@ -4228,10 +4242,10 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="59" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="B62" s="59" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="59"/>
@@ -4253,24 +4267,24 @@
         <v>20</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C63" s="58"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B64" s="58" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="C65" s="58"/>
       <c r="D65" s="58"/>
@@ -4281,10 +4295,10 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="C66" s="58"/>
       <c r="D66" s="58"/>
@@ -4293,10 +4307,10 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B67" s="58" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="C67" s="58"/>
       <c r="D67" s="58"/>
@@ -4308,20 +4322,20 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B68" s="58" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="C68" s="58"/>
       <c r="D68" s="58"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B69" s="58" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="C69" s="58"/>
       <c r="D69" s="58"/>
@@ -4330,10 +4344,10 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B70" s="58" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="C70" s="58"/>
       <c r="D70" s="58"/>
@@ -4343,10 +4357,10 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" s="59" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="B72" s="59" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="C72" s="59"/>
       <c r="D72" s="59"/>
@@ -4354,30 +4368,30 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" s="39" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="B73" s="58" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="C73" s="58"/>
       <c r="D73" s="58"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" s="39" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="B74" s="58" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="C74" s="58"/>
       <c r="D74" s="58"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A75" s="39" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="B75" s="58" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C75" s="58"/>
       <c r="D75" s="58"/>
@@ -4385,10 +4399,10 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" s="39" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="C76" s="58"/>
       <c r="D76" s="58"/>
@@ -4405,10 +4419,10 @@
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A77" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B77" s="58" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C77" s="58"/>
       <c r="D77" s="58"/>
@@ -4442,10 +4456,10 @@
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A78" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B78" s="58" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="C78" s="58"/>
       <c r="D78" s="58"/>
@@ -4467,10 +4481,10 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A79" s="39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B79" s="58" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="C79" s="58"/>
       <c r="D79" s="58"/>
@@ -4488,10 +4502,10 @@
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A80" s="39" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="C80" s="58"/>
       <c r="D80" s="58"/>
@@ -4506,10 +4520,10 @@
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B81" s="58" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="C81" s="58"/>
       <c r="D81" s="58"/>
@@ -4526,10 +4540,10 @@
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="39" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B82" s="58" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="C82" s="58"/>
       <c r="D82" s="58"/>
@@ -4544,10 +4558,10 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="39" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B83" s="58" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="C83" s="58"/>
       <c r="D83" s="58"/>
@@ -4564,10 +4578,10 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="39" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B84" s="58" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C84" s="58"/>
       <c r="D84" s="58"/>
@@ -4594,10 +4608,10 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="39" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="B85" s="58" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="C85" s="58"/>
       <c r="D85" s="58"/>
@@ -4606,10 +4620,10 @@
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="39" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="B86" s="58" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="C86" s="58"/>
       <c r="D86" s="58"/>
@@ -4620,10 +4634,10 @@
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="39" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="B87" s="58" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="C87" s="58"/>
       <c r="D87" s="58"/>
@@ -4631,10 +4645,10 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="39" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B88" s="58" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="C88" s="58"/>
       <c r="D88" s="58"/>
@@ -4642,10 +4656,10 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="39" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="B89" s="58" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="C89" s="58"/>
       <c r="D89" s="58"/>
@@ -4653,58 +4667,58 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="39" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="B90" s="58" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="C90" s="58"/>
       <c r="D90" s="58"/>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="39" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="B91" s="58" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="C91" s="58"/>
       <c r="D91" s="58"/>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="39" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="B92" s="58" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="C92" s="58"/>
       <c r="D92" s="58"/>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="39" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="B93" s="58" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="C93" s="58"/>
       <c r="D93" s="58"/>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="39" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="39" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="B95" s="58" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="C95" s="58"/>
       <c r="D95" s="58"/>
@@ -4718,10 +4732,10 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="39" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B96" s="58" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="C96" s="58"/>
       <c r="D96" s="58"/>
@@ -4742,10 +4756,10 @@
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="39" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="B97" s="58" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C97" s="58"/>
       <c r="D97" s="58"/>
@@ -4756,10 +4770,10 @@
     </row>
     <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="39" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="B98" s="58" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="C98" s="58"/>
       <c r="D98" s="58"/>
@@ -4777,10 +4791,10 @@
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="39" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B99" s="58" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="C99" s="58"/>
       <c r="D99" s="58"/>
@@ -4802,15 +4816,15 @@
     </row>
     <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="59" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="39" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B102" s="58" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="C102" s="58"/>
       <c r="D102" s="58"/>
@@ -4834,10 +4848,10 @@
     </row>
     <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B103" s="58" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="C103" s="58"/>
       <c r="D103" s="58"/>
@@ -4862,10 +4876,10 @@
     </row>
     <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B104" s="58" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="C104" s="58"/>
       <c r="D104" s="58"/>
@@ -4898,10 +4912,10 @@
     </row>
     <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B105" s="58" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="C105" s="58"/>
       <c r="D105" s="58"/>
@@ -4931,10 +4945,10 @@
     </row>
     <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B106" s="58" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="C106" s="58"/>
       <c r="D106" s="58"/>
@@ -4954,10 +4968,10 @@
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B107" s="58" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="C107" s="58"/>
       <c r="D107" s="58"/>
@@ -4978,10 +4992,10 @@
     </row>
     <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" s="39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B108" s="58" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="C108" s="58"/>
       <c r="D108" s="58"/>
@@ -5011,7 +5025,7 @@
     </row>
     <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" s="59" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B110" s="59" t="s">
         <v>17</v>
@@ -5019,7 +5033,7 @@
     </row>
     <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" s="59" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B112" s="59"/>
     </row>
@@ -5028,7 +5042,7 @@
         <v>20</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C113" s="58"/>
       <c r="D113" s="58"/>
@@ -5053,10 +5067,10 @@
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114" s="39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B114" s="58" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="C114" s="58"/>
       <c r="D114" s="58"/>
@@ -5077,10 +5091,10 @@
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115" s="39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B115" s="58" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="C115" s="58"/>
       <c r="D115" s="58"/>
@@ -5115,8 +5129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76F439B-9760-4E2D-9273-BA22847E3391}">
   <dimension ref="A1:AD63"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A3:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5147,96 +5161,96 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B1" s="27">
         <f>DataSheet!D6</f>
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="R3" s="30" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="S3" s="72" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="U3" s="31" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -6294,7 +6308,7 @@
         <v>51.000000000000078</v>
       </c>
       <c r="W15" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="X15" cm="1">
         <f t="array" ref="X15">_xlfn.IFS(B1=0,X12-X13,B1=1,X7-X8)</f>
@@ -6382,7 +6396,7 @@
         <v>34.999999999999929</v>
       </c>
       <c r="W16" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -6462,7 +6476,7 @@
         <v>50.000000000000036</v>
       </c>
       <c r="W17" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -6662,33 +6676,33 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="R24" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="K27" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.25">
@@ -6794,6 +6808,474 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34519FF6-6B75-48A6-9D4D-DC0EEC67962C}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="79">
+        <v>44254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="79">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="79">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="79">
+        <v>44257</v>
+      </c>
+      <c r="B5" s="81">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C5" s="81">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H5" s="81">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="79">
+        <v>44258</v>
+      </c>
+      <c r="B6" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="C6" s="81">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H6" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="79">
+        <v>44259</v>
+      </c>
+      <c r="B7" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="C7" s="81">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H7" s="81">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="79">
+        <v>44260</v>
+      </c>
+      <c r="B8" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="C8" s="81">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H8" s="81">
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="79">
+        <v>44261</v>
+      </c>
+      <c r="B9" s="81">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C9" s="81">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H9" s="81">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="79">
+        <v>44262</v>
+      </c>
+      <c r="B10" s="81">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="C10" s="81">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H10" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="79">
+        <v>44263</v>
+      </c>
+      <c r="B11" s="81">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C11" s="81">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="81">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H11" s="81">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="79">
+        <v>44264</v>
+      </c>
+      <c r="B12" s="81">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="C12" s="81">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="81">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H12" s="81">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="79">
+        <v>44265</v>
+      </c>
+      <c r="B13" s="81">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C13" s="81">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" s="81">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H13" s="81">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="79">
+        <v>44266</v>
+      </c>
+      <c r="B14" s="81">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C14" s="81">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="81">
+        <v>0.3125</v>
+      </c>
+      <c r="H14" s="81">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="79">
+        <v>44267</v>
+      </c>
+      <c r="B15" s="81">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C15" s="81">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15" s="81">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="H15" s="81">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="79">
+        <v>44268</v>
+      </c>
+      <c r="B16" s="81">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="81">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" s="81">
+        <v>0.29930555555555555</v>
+      </c>
+      <c r="H16" s="81">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="79">
+        <v>44269</v>
+      </c>
+      <c r="B17" s="81">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C17" s="81">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="81">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H17" s="81">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="79">
+        <v>44270</v>
+      </c>
+      <c r="B18" s="81">
+        <v>0.96875</v>
+      </c>
+      <c r="C18" s="81">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="81">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H18" s="81">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A0A131-AB0B-48E7-BA89-4CA72DAFD876}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -6815,7 +7297,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -6824,7 +7306,7 @@
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
       <c r="I1" s="25" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="J1" s="25"/>
       <c r="K1" s="25"/>
@@ -6835,16 +7317,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="M2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6893,7 +7375,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>20</v>
@@ -6902,7 +7384,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>20</v>
@@ -6911,7 +7393,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>20</v>
@@ -6920,12 +7402,12 @@
         <v>3</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="15">
         <v>1</v>
@@ -6935,7 +7417,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="15">
         <v>1</v>
@@ -6945,7 +7427,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="15">
         <v>1</v>
@@ -6955,7 +7437,7 @@
         <v>34</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N5" s="15">
         <v>1</v>
@@ -6967,25 +7449,25 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="15">
         <v>1</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6" s="15">
         <v>1</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N6" s="15">
         <v>1</v>
@@ -6993,45 +7475,45 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J7" s="15">
         <v>1</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>29</v>
-      </c>
       <c r="N7" s="15">
         <v>1</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="15">
         <v>2</v>
@@ -7041,7 +7523,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
@@ -7051,7 +7533,7 @@
         <v>11</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J8" s="15">
         <v>3</v>
@@ -7061,7 +7543,7 @@
         <v>11</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N8" s="15">
         <v>2</v>
@@ -7073,25 +7555,25 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F9" s="15">
         <v>1</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J9" s="15">
         <v>1</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="N9" s="15">
         <v>1</v>
@@ -7099,25 +7581,25 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F10" s="15">
         <v>1</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J10" s="15">
         <v>1</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N10" s="15">
         <v>1</v>
@@ -7125,25 +7607,25 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B11" s="15">
         <v>1</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F11" s="15">
         <v>1</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J11" s="15">
         <v>1</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N11" s="15">
         <v>1</v>
@@ -7151,25 +7633,25 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B12" s="15">
         <v>3</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F12" s="15">
         <v>3</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J12" s="15">
         <v>5</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="N12" s="15">
         <v>5</v>
@@ -7177,25 +7659,25 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B13" s="15">
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F13" s="15">
         <v>2</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J13" s="15">
         <v>4</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="N13" s="15">
         <v>4</v>
@@ -7203,25 +7685,25 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B14" s="15">
         <v>2</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F14" s="15">
         <v>2</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J14" s="15">
         <v>1</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="N14" s="15">
         <v>1</v>
@@ -7229,25 +7711,25 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F15" s="15">
         <v>1</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J15" s="15">
         <v>4</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N15" s="15">
         <v>4</v>
@@ -7255,25 +7737,25 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B16" s="15">
         <v>3</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F16" s="15">
         <v>1</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J16" s="15">
         <v>1</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="N16" s="15">
         <v>1</v>
@@ -7281,25 +7763,25 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B17" s="15">
         <v>1</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F17" s="15">
         <v>2</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="J17" s="15">
         <v>3</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N17" s="15">
         <v>2</v>
@@ -7307,25 +7789,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B18" s="15">
         <v>2</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F18" s="15">
         <v>1</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J18" s="15">
         <v>2</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N18" s="15">
         <v>1</v>
@@ -7333,25 +7815,25 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B19" s="15">
         <v>5</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F19" s="15">
         <v>5</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="J19" s="15">
         <v>4</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="N19" s="15">
         <v>3</v>
@@ -7359,25 +7841,25 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B20" s="15">
         <v>2</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F20" s="15">
         <v>2</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="J20" s="15">
         <v>4</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="N20" s="15">
         <v>4</v>
@@ -7385,25 +7867,25 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B21" s="15">
         <v>1</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F21" s="15">
         <v>1</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="J21" s="15">
         <v>1</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="N21" s="15">
         <v>1</v>
@@ -7411,25 +7893,25 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B22" s="15">
         <v>1</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="J22" s="15">
         <v>3</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="N22" s="15">
         <v>2</v>
@@ -7437,25 +7919,25 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B23" s="15">
         <v>1</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F23" s="15">
         <v>1</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="J23" s="15">
         <v>1</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="N23" s="15">
         <v>1</v>
@@ -7466,12 +7948,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA813570-53F3-4A84-BAEE-DE1DA48FE075}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7481,17 +7963,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
@@ -7504,12 +7986,12 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="61"/>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
@@ -7524,12 +8006,12 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
@@ -7544,17 +8026,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
@@ -7563,7 +8045,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="53"/>
@@ -7575,7 +8057,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -7584,7 +8066,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
@@ -7596,7 +8078,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="73" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B15" s="74"/>
       <c r="C15" s="74"/>
@@ -7607,7 +8089,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="B16" s="53"/>
       <c r="C16" s="53"/>
@@ -7619,14 +8101,14 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="73" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B17" s="74"/>
       <c r="C17" s="75"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -7638,7 +8120,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="B20" s="15">
         <v>0</v>
@@ -7646,23 +8128,23 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="B21" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
@@ -7675,12 +8157,12 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
@@ -7695,12 +8177,12 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
@@ -7715,17 +8197,17 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
@@ -7734,7 +8216,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="B35" s="53"/>
       <c r="C35" s="53"/>
@@ -7746,7 +8228,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="73" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="B36" s="74"/>
       <c r="C36" s="74"/>
@@ -7755,7 +8237,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
@@ -7767,7 +8249,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="73" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B38" s="74"/>
       <c r="C38" s="74"/>
@@ -7778,7 +8260,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="52" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -7790,7 +8272,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="73" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B40" s="74"/>
       <c r="C40" s="75"/>
@@ -7807,7 +8289,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="B43" s="15">
         <v>1</v>
@@ -7815,7 +8297,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="B44" s="15">
         <v>5</v>

</xml_diff>